<commit_message>
data archive for publication
</commit_message>
<xml_diff>
--- a/data/data_raw/from_collectors/jean_raw_data_2021.xlsx
+++ b/data/data_raw/from_collectors/jean_raw_data_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjean\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmola/My Drive/Work/Colorado State University/Projects/rpbb_popgen_archive/data/data_raw/from_collectors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E86A945D-4C45-41D8-94F5-E3A2D45C3A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E51C030D-CB82-7C4B-BEF9-BCADBF1B0AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7360" xr2:uid="{5CB17538-D19C-459D-B303-0A6443B2327B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{5CB17538-D19C-459D-B303-0A6443B2327B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,7 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,13 +206,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -238,10 +231,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,29 +551,28 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD1048576"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +622,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -651,10 +642,10 @@
         <v>37</v>
       </c>
       <c r="G2">
-        <v>41.921926999999997</v>
+        <v>41.925926999999994</v>
       </c>
       <c r="H2">
-        <v>-89.351540999999997</v>
+        <v>-89.349541000000002</v>
       </c>
       <c r="I2" t="s">
         <v>39</v>
@@ -678,7 +669,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -698,10 +689,10 @@
         <v>37</v>
       </c>
       <c r="G3">
-        <v>41.921928999999999</v>
+        <v>41.923929000000001</v>
       </c>
       <c r="H3">
-        <v>-89.351551000000001</v>
+        <v>-89.346551000000005</v>
       </c>
       <c r="I3" t="s">
         <v>39</v>
@@ -725,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -745,10 +736,10 @@
         <v>38</v>
       </c>
       <c r="G4">
-        <v>41.887827999999999</v>
+        <v>41.892828000000002</v>
       </c>
       <c r="H4">
-        <v>-89.368168999999995</v>
+        <v>-89.366168999999999</v>
       </c>
       <c r="I4" t="s">
         <v>39</v>
@@ -772,7 +763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -791,11 +782,11 @@
       <c r="F5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="2">
-        <v>43.611919</v>
-      </c>
-      <c r="H5" s="2">
-        <v>-89.26576</v>
+      <c r="G5">
+        <v>43.616919000000003</v>
+      </c>
+      <c r="H5">
+        <v>-89.260760000000005</v>
       </c>
       <c r="I5" t="s">
         <v>43</v>
@@ -819,7 +810,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -838,11 +829,11 @@
       <c r="F6" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="2">
-        <v>43.696061999999998</v>
-      </c>
-      <c r="H6" s="2">
-        <v>-89.399114999999995</v>
+      <c r="G6">
+        <v>43.699061999999998</v>
+      </c>
+      <c r="H6">
+        <v>-89.396114999999995</v>
       </c>
       <c r="I6" t="s">
         <v>43</v>
@@ -866,7 +857,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -885,11 +876,11 @@
       <c r="F7" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="2">
-        <v>43.695906000000001</v>
-      </c>
-      <c r="H7" s="2">
-        <v>-89.398875000000004</v>
+      <c r="G7">
+        <v>43.699905999999999</v>
+      </c>
+      <c r="H7">
+        <v>-89.394874999999999</v>
       </c>
       <c r="I7" t="s">
         <v>43</v>
@@ -913,7 +904,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -932,11 +923,11 @@
       <c r="F8" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="2">
-        <v>43.696953999999998</v>
-      </c>
-      <c r="H8" s="2">
-        <v>-89.389244000000005</v>
+      <c r="G8">
+        <v>43.699953999999998</v>
+      </c>
+      <c r="H8">
+        <v>-89.38424400000001</v>
       </c>
       <c r="I8" t="s">
         <v>43</v>
@@ -960,7 +951,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -979,11 +970,11 @@
       <c r="F9" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="2">
-        <v>43.696192000000003</v>
-      </c>
-      <c r="H9" s="2">
-        <v>-89.389836000000003</v>
+      <c r="G9">
+        <v>43.699192000000004</v>
+      </c>
+      <c r="H9">
+        <v>-89.385835999999998</v>
       </c>
       <c r="I9" t="s">
         <v>43</v>
@@ -1007,7 +998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1026,11 +1017,11 @@
       <c r="F10" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="2">
-        <v>43.611513000000002</v>
-      </c>
-      <c r="H10" s="2">
-        <v>-89.264359999999996</v>
+      <c r="G10">
+        <v>43.613513000000005</v>
+      </c>
+      <c r="H10">
+        <v>-89.261359999999996</v>
       </c>
       <c r="I10" t="s">
         <v>43</v>
@@ -1054,7 +1045,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1073,11 +1064,11 @@
       <c r="F11" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="2">
-        <v>43.610748000000001</v>
-      </c>
-      <c r="H11" s="2">
-        <v>-89.260880999999998</v>
+      <c r="G11">
+        <v>43.614747999999999</v>
+      </c>
+      <c r="H11">
+        <v>-89.258881000000002</v>
       </c>
       <c r="I11" t="s">
         <v>43</v>

</xml_diff>